<commit_message>
Update IP assignments spreadsheet
</commit_message>
<xml_diff>
--- a/ip assignments.xlsx
+++ b/ip assignments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Projects\infrastructure-vm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brad\Foundry\infrastructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF84008-7BDC-4D62-8AF9-A863E46218F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563DA480-3C47-49B5-B4F3-DD9D30BB2BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
   </bookViews>
   <sheets>
     <sheet name="hosts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="474">
   <si>
     <t>#</t>
   </si>
@@ -1436,6 +1436,12 @@
   </si>
   <si>
     <t>wwquicksilver2</t>
+  </si>
+  <si>
+    <t>192.168.0.23</t>
+  </si>
+  <si>
+    <t>nfs1</t>
   </si>
 </sst>
 </file>
@@ -2327,33 +2333,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F389"/>
+  <dimension ref="A1:F390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="H114" sqref="H114"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.109375" style="1"/>
     <col min="4" max="4" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="15.5703125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="9.109375" style="1"/>
+    <col min="12" max="12" width="15.5546875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>447</v>
       </c>
@@ -2361,7 +2367,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>449</v>
       </c>
@@ -2369,7 +2375,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>451</v>
       </c>
@@ -2377,7 +2383,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>453</v>
       </c>
@@ -2385,7 +2391,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>455</v>
       </c>
@@ -2393,7 +2399,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>457</v>
       </c>
@@ -2401,7 +2407,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>459</v>
       </c>
@@ -2409,7 +2415,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>180</v>
       </c>
@@ -2417,7 +2423,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>189</v>
       </c>
@@ -2425,7 +2431,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>103</v>
       </c>
@@ -2437,7 +2443,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2451,7 +2457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -2465,7 +2471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -2482,7 +2488,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
@@ -2499,7 +2505,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -2516,7 +2522,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -2533,7 +2539,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -2550,7 +2556,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -2567,7 +2573,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -2584,7 +2590,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
@@ -2601,7 +2607,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
@@ -2618,7 +2624,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
@@ -2635,7 +2641,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
@@ -2652,7 +2658,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
@@ -2669,7 +2675,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
@@ -2686,7 +2692,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
@@ -2703,7 +2709,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>54</v>
       </c>
@@ -2720,7 +2726,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>79</v>
       </c>
@@ -2737,7 +2743,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
@@ -2751,7 +2757,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -2765,7 +2771,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
@@ -2779,7 +2785,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>87</v>
       </c>
@@ -2793,7 +2799,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>88</v>
       </c>
@@ -2807,7 +2813,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>89</v>
       </c>
@@ -2821,7 +2827,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>90</v>
       </c>
@@ -2835,7 +2841,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>465</v>
       </c>
@@ -2849,7 +2855,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>466</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>27</v>
       </c>
@@ -2877,7 +2883,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>29</v>
       </c>
@@ -2891,7 +2897,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>31</v>
       </c>
@@ -2905,7 +2911,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>33</v>
       </c>
@@ -2919,7 +2925,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>34</v>
       </c>
@@ -2933,7 +2939,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>35</v>
       </c>
@@ -2947,7 +2953,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>37</v>
       </c>
@@ -2961,7 +2967,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>39</v>
       </c>
@@ -2975,7 +2981,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>41</v>
       </c>
@@ -2989,7 +2995,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
@@ -3003,7 +3009,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
@@ -3017,7 +3023,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>81</v>
       </c>
@@ -3031,7 +3037,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -3045,7 +3051,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>74</v>
       </c>
@@ -3059,7 +3065,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
@@ -3073,7 +3079,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>104</v>
       </c>
@@ -3087,7 +3093,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>68</v>
       </c>
@@ -3101,7 +3107,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>69</v>
       </c>
@@ -3115,7 +3121,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>70</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>99</v>
       </c>
@@ -3137,7 +3143,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>71</v>
       </c>
@@ -3145,7 +3151,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>72</v>
       </c>
@@ -3153,7 +3159,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>73</v>
       </c>
@@ -3161,1834 +3167,1848 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E73" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E74" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E79" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="E80" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E81" s="1" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E82" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D82" s="1" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D83" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="E83" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D83" s="1" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D84" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E84" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D84" s="1" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D85" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E85" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D85" s="1" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D86" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E86" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D86" s="1" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D87" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="E87" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D87" s="1" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D88" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="E88" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D88" s="1" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D89" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E89" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D89" s="1" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D90" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="E90" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D90" s="1" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D91" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="E91" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D91" s="1" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D92" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E92" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D92" s="1" t="s">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D93" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="E93" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D93" s="1" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D94" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="E94" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D94" s="1" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D95" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="E95" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D95" s="1" t="s">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D96" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="E96" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D96" s="1" t="s">
+    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D97" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D97" s="1" t="s">
+    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D98" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="E98" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D98" s="1" t="s">
+    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D99" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="E99" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D99" s="1" t="s">
+    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D100" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="E100" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D100" s="1" t="s">
+    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D101" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E100" s="1" t="s">
+      <c r="E101" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="101" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D101" s="1" t="s">
+    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D102" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="E102" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="102" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D102" s="1" t="s">
+    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D103" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E102" s="1" t="s">
+      <c r="E103" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D103" s="1" t="s">
+    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D104" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E103" s="1" t="s">
+      <c r="E104" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D104" s="1" t="s">
+    <row r="105" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D105" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="E105" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="105" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D105" s="1" t="s">
+    <row r="106" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D106" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E105" s="1" t="s">
+      <c r="E106" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="107" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D107" s="1" t="s">
+    <row r="108" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D108" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E107" s="1" t="s">
+      <c r="E108" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D108" s="1" t="s">
+    <row r="109" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D109" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="E109" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="109" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D109" s="1" t="s">
+    <row r="110" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D110" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E109" s="1" t="s">
+      <c r="E110" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="110" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D110" s="1" t="s">
+    <row r="111" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D111" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E110" s="1" t="s">
+      <c r="E111" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D114" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E113" s="1" t="s">
+      <c r="E114" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115" s="1" t="s">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B116" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="E116" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E116" s="1" t="s">
+      <c r="E117" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B118" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D118" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E117" s="1" t="s">
+      <c r="E118" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B119" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D119" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="E119" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B120" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E119" s="1" t="s">
+      <c r="E120" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E120" s="1" t="s">
+      <c r="E121" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B122" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D122" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E121" s="1" t="s">
+      <c r="E122" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B123" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="D123" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E122" s="1" t="s">
+      <c r="E123" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B124" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D124" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E123" s="1" t="s">
+      <c r="E124" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A124" s="1" t="s">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B125" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D125" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E124" s="1" t="s">
+      <c r="E125" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125" s="1" t="s">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B126" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D126" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E125" s="1" t="s">
+      <c r="E126" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="D127" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128" s="1" t="s">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="D129" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A129" s="1" t="s">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B130" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D129" s="1" t="s">
+      <c r="D130" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A130" s="1" t="s">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B131" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="D131" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E130" s="1" t="s">
+      <c r="E131" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
+    <row r="135" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A135" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B135" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
+    <row r="136" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A136" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B136" s="1" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
+    <row r="137" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A137" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B137" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B138" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B139" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A139" s="1" t="s">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B140" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A140" s="1" t="s">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A141" s="1" t="s">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A142" s="1" t="s">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A143" s="1" t="s">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A144" s="1" t="s">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A145" s="1" t="s">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A146" s="1" t="s">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A147" s="1" t="s">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A148" s="1" t="s">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A149" s="1" t="s">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A150" s="1" t="s">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A151" s="1" t="s">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A152" s="1" t="s">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A153" s="1" t="s">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A154" s="1" t="s">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A155" s="1" t="s">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A156" s="1" t="s">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A157" s="1" t="s">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A158" s="1" t="s">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A159" s="1" t="s">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A160" s="1" t="s">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A161" s="1" t="s">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A162" s="1" t="s">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A163" s="1" t="s">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A164" s="1" t="s">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A165" s="1" t="s">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A166" s="1" t="s">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A167" s="1" t="s">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A168" s="1" t="s">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A169" s="1" t="s">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A170" s="1" t="s">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A171" s="1" t="s">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A172" s="1" t="s">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A173" s="1" t="s">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A174" s="1" t="s">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A175" s="1" t="s">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A176" s="1" t="s">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A177" s="1" t="s">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A178" s="1" t="s">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A179" s="1" t="s">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A180" s="1" t="s">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A181" s="1" t="s">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A182" s="1" t="s">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A183" s="1" t="s">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A184" s="1" t="s">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A185" s="1" t="s">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A186" s="1" t="s">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A187" s="1" t="s">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A188" s="1" t="s">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A189" s="1" t="s">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A190" s="1" t="s">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A191" s="1" t="s">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A192" s="1" t="s">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A193" s="1" t="s">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A194" s="1" t="s">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A195" s="1" t="s">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A196" s="1" t="s">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A197" s="1" t="s">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A198" s="1" t="s">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A199" s="1" t="s">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A200" s="1" t="s">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A201" s="1" t="s">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A202" s="1" t="s">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A203" s="1" t="s">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A204" s="1" t="s">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A205" s="1" t="s">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A206" s="1" t="s">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A207" s="1" t="s">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A208" s="1" t="s">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A209" s="1" t="s">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A210" s="1" t="s">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A211" s="1" t="s">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A212" s="1" t="s">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A213" s="1" t="s">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A214" s="1" t="s">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A215" s="1" t="s">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A216" s="1" t="s">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A217" s="1" t="s">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A218" s="1" t="s">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A219" s="1" t="s">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A220" s="1" t="s">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A221" s="1" t="s">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A222" s="1" t="s">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A223" s="1" t="s">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A224" s="1" t="s">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A225" s="1" t="s">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A226" s="1" t="s">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A227" s="1" t="s">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A228" s="1" t="s">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A229" s="1" t="s">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A230" s="1" t="s">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A231" s="1" t="s">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A232" s="1" t="s">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A233" s="1" t="s">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A234" s="1" t="s">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A235" s="1" t="s">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A236" s="1" t="s">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A237" s="1" t="s">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A238" s="1" t="s">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A239" s="1" t="s">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A240" s="1" t="s">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A241" s="1" t="s">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A242" s="1" t="s">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A243" s="1" t="s">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A244" s="1" t="s">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A245" s="1" t="s">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A246" s="1" t="s">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A247" s="1" t="s">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A248" s="1" t="s">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A249" s="1" t="s">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A250" s="1" t="s">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A251" s="1" t="s">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A252" s="1" t="s">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A253" s="1" t="s">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A254" s="1" t="s">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A255" s="1" t="s">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A256" s="1" t="s">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A257" s="1" t="s">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A258" s="1" t="s">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A259" s="1" t="s">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A260" s="1" t="s">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A261" s="1" t="s">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A262" s="1" t="s">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A263" s="1" t="s">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A264" s="1" t="s">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A265" s="1" t="s">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A266" s="1" t="s">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A267" s="1" t="s">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A268" s="1" t="s">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A269" s="1" t="s">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A270" s="1" t="s">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A271" s="1" t="s">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A272" s="1" t="s">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A273" s="1" t="s">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A274" s="1" t="s">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A275" s="1" t="s">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A276" s="1" t="s">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A277" s="1" t="s">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A278" s="1" t="s">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A279" s="1" t="s">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A280" s="1" t="s">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A281" s="1" t="s">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A282" s="1" t="s">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A283" s="1" t="s">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A284" s="1" t="s">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="1" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A285" s="1" t="s">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A286" s="1" t="s">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A287" s="1" t="s">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A288" s="1" t="s">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="1" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A289" s="1" t="s">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="1" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A290" s="1" t="s">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A291" s="1" t="s">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A292" s="1" t="s">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A293" s="1" t="s">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="1" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A294" s="1" t="s">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="1" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A295" s="1" t="s">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="1" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A296" s="1" t="s">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A297" s="1" t="s">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A298" s="1" t="s">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A299" s="1" t="s">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A300" s="1" t="s">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="1" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A301" s="1" t="s">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A302" s="1" t="s">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="1" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A303" s="1" t="s">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" s="1" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A304" s="1" t="s">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A305" s="1" t="s">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A306" s="1" t="s">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A307" s="1" t="s">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A308" s="1" t="s">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A309" s="1" t="s">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A310" s="1" t="s">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A311" s="1" t="s">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A312" s="1" t="s">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A313" s="1" t="s">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A314" s="1" t="s">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="1" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A315" s="1" t="s">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" s="1" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A316" s="1" t="s">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" s="1" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A317" s="1" t="s">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A318" s="1" t="s">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" s="1" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A319" s="1" t="s">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" s="1" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A320" s="1" t="s">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A321" s="1" t="s">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" s="1" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A322" s="1" t="s">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" s="1" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A323" s="1" t="s">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A324" s="1" t="s">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" s="1" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A325" s="1" t="s">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" s="1" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A326" s="1" t="s">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" s="1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A327" s="1" t="s">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A328" s="1" t="s">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A329" s="1" t="s">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A330" s="1" t="s">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A331" s="1" t="s">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A332" s="1" t="s">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A333" s="1" t="s">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" s="1" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A334" s="1" t="s">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" s="1" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A335" s="1" t="s">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" s="1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A336" s="1" t="s">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A337" s="1" t="s">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A338" s="1" t="s">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A339" s="1" t="s">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" s="1" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A340" s="1" t="s">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A341" s="1" t="s">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A342" s="1" t="s">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A343" s="1" t="s">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" s="1" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A344" s="1" t="s">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A345" s="1" t="s">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A346" s="1" t="s">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" s="1" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A347" s="1" t="s">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A348" s="1" t="s">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A349" s="1" t="s">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A350" s="1" t="s">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" s="1" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A351" s="1" t="s">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" s="1" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A352" s="1" t="s">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A353" s="1" t="s">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" s="1" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A354" s="1" t="s">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A355" s="1" t="s">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" s="1" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A356" s="1" t="s">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" s="1" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A357" s="1" t="s">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" s="1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A358" s="1" t="s">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A359" s="1" t="s">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A360" s="1" t="s">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A361" s="1" t="s">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A362" s="1" t="s">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" s="1" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A363" s="1" t="s">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" s="1" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A364" s="1" t="s">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" s="1" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A365" s="1" t="s">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" s="1" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A366" s="1" t="s">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" s="1" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A367" s="1" t="s">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" s="1" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A368" s="1" t="s">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" s="1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A369" s="1" t="s">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" s="1" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A370" s="1" t="s">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" s="1" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A371" s="1" t="s">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A372" s="1" t="s">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" s="1" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A373" s="1" t="s">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A374" s="1" t="s">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A375" s="1" t="s">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A376" s="1" t="s">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A377" s="1" t="s">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" s="1" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A378" s="1" t="s">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A379" s="1" t="s">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A380" s="1" t="s">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" s="1" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A381" s="1" t="s">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" s="1" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A382" s="1" t="s">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A383" s="1" t="s">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" s="1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A384" s="1" t="s">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" s="1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A385" s="1" t="s">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A386" s="1" t="s">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A387" s="1" t="s">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" s="1" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A388" s="1" t="s">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A389" s="1" t="s">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" s="1" t="s">
         <v>444</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance webhook script with improved response logging and error handling; ensure proper handling of success and failure states.
</commit_message>
<xml_diff>
--- a/ip assignments.xlsx
+++ b/ip assignments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brad\Foundry\infrastructure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Foundry\infrastructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563DA480-3C47-49B5-B4F3-DD9D30BB2BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB88E2BD-9CDA-4C3E-93FE-765DFA899546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
   </bookViews>
   <sheets>
     <sheet name="hosts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="473">
   <si>
     <t>#</t>
   </si>
@@ -1432,16 +1432,13 @@
     <t>10.20.20..61</t>
   </si>
   <si>
-    <t>wwquicksilver.vm.local</t>
-  </si>
-  <si>
-    <t>wwquicksilver2</t>
-  </si>
-  <si>
     <t>192.168.0.23</t>
   </si>
   <si>
     <t>nfs1</t>
+  </si>
+  <si>
+    <t>test pod</t>
   </si>
 </sst>
 </file>
@@ -2335,31 +2332,31 @@
   </sheetPr>
   <dimension ref="A1:F390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="9.109375" style="1"/>
-    <col min="12" max="12" width="15.5546875" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="1"/>
+    <col min="6" max="6" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="15.5703125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>447</v>
       </c>
@@ -2367,7 +2364,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>449</v>
       </c>
@@ -2375,7 +2372,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>451</v>
       </c>
@@ -2383,7 +2380,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>453</v>
       </c>
@@ -2391,7 +2388,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>455</v>
       </c>
@@ -2399,7 +2396,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>457</v>
       </c>
@@ -2407,7 +2404,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>459</v>
       </c>
@@ -2415,7 +2412,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>180</v>
       </c>
@@ -2423,7 +2420,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>189</v>
       </c>
@@ -2431,7 +2428,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>103</v>
       </c>
@@ -2443,7 +2440,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2457,7 +2454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -2471,7 +2468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -2488,7 +2485,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
@@ -2505,7 +2502,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -2522,7 +2519,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -2539,7 +2536,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -2556,7 +2553,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -2573,7 +2570,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -2590,7 +2587,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
@@ -2607,7 +2604,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
@@ -2624,7 +2621,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
@@ -2641,7 +2638,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
@@ -2658,7 +2655,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
@@ -2675,7 +2672,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
@@ -2692,7 +2689,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
@@ -2709,7 +2706,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>54</v>
       </c>
@@ -2726,7 +2723,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>79</v>
       </c>
@@ -2743,7 +2740,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
@@ -2757,7 +2754,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -2771,7 +2768,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
@@ -2785,7 +2782,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>87</v>
       </c>
@@ -2799,7 +2796,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>88</v>
       </c>
@@ -2813,7 +2810,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>89</v>
       </c>
@@ -2827,7 +2824,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>90</v>
       </c>
@@ -2841,7 +2838,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>465</v>
       </c>
@@ -2855,7 +2852,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>466</v>
       </c>
@@ -2869,7 +2866,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>27</v>
       </c>
@@ -2883,7 +2880,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>29</v>
       </c>
@@ -2897,7 +2894,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>31</v>
       </c>
@@ -2911,7 +2908,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>33</v>
       </c>
@@ -2925,7 +2922,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>34</v>
       </c>
@@ -2939,7 +2936,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>35</v>
       </c>
@@ -2953,7 +2950,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>37</v>
       </c>
@@ -2967,7 +2964,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>39</v>
       </c>
@@ -2981,7 +2978,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>41</v>
       </c>
@@ -2995,7 +2992,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
@@ -3009,7 +3006,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
@@ -3023,7 +3020,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>81</v>
       </c>
@@ -3037,7 +3034,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -3051,7 +3048,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>74</v>
       </c>
@@ -3065,7 +3062,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
@@ -3079,7 +3076,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>104</v>
       </c>
@@ -3093,7 +3090,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>68</v>
       </c>
@@ -3107,7 +3104,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>69</v>
       </c>
@@ -3121,7 +3118,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>70</v>
       </c>
@@ -3129,7 +3126,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>99</v>
       </c>
@@ -3143,7 +3140,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>71</v>
       </c>
@@ -3151,7 +3148,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>72</v>
       </c>
@@ -3159,7 +3156,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>73</v>
       </c>
@@ -3167,21 +3164,21 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>182</v>
       </c>
@@ -3195,7 +3192,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>183</v>
       </c>
@@ -3209,7 +3206,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>105</v>
       </c>
@@ -3217,7 +3214,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>185</v>
       </c>
@@ -3231,7 +3228,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>159</v>
       </c>
@@ -3245,21 +3242,15 @@
         <v>160</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>470</v>
-      </c>
       <c r="D81" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="E81" s="1" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>109</v>
       </c>
@@ -3273,7 +3264,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D83" s="1" t="s">
         <v>130</v>
       </c>
@@ -3281,7 +3272,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D84" s="1" t="s">
         <v>131</v>
       </c>
@@ -3289,7 +3280,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D85" s="1" t="s">
         <v>132</v>
       </c>
@@ -3297,7 +3288,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D86" s="1" t="s">
         <v>133</v>
       </c>
@@ -3305,7 +3296,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D87" s="1" t="s">
         <v>134</v>
       </c>
@@ -3313,7 +3304,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D88" s="1" t="s">
         <v>135</v>
       </c>
@@ -3321,7 +3312,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D89" s="1" t="s">
         <v>136</v>
       </c>
@@ -3329,7 +3320,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D90" s="1" t="s">
         <v>137</v>
       </c>
@@ -3337,7 +3328,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D91" s="1" t="s">
         <v>138</v>
       </c>
@@ -3345,7 +3336,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D92" s="1" t="s">
         <v>139</v>
       </c>
@@ -3353,7 +3344,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D93" s="1" t="s">
         <v>140</v>
       </c>
@@ -3361,7 +3352,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D94" s="1" t="s">
         <v>141</v>
       </c>
@@ -3369,7 +3360,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D95" s="1" t="s">
         <v>142</v>
       </c>
@@ -3377,7 +3368,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D96" s="1" t="s">
         <v>143</v>
       </c>
@@ -3385,7 +3376,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D97" s="1" t="s">
         <v>144</v>
       </c>
@@ -3393,7 +3384,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D98" s="1" t="s">
         <v>145</v>
       </c>
@@ -3401,7 +3392,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D99" s="1" t="s">
         <v>146</v>
       </c>
@@ -3409,7 +3400,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D100" s="1" t="s">
         <v>147</v>
       </c>
@@ -3417,7 +3408,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D101" s="1" t="s">
         <v>148</v>
       </c>
@@ -3425,7 +3416,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D102" s="1" t="s">
         <v>149</v>
       </c>
@@ -3433,7 +3424,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D103" s="1" t="s">
         <v>150</v>
       </c>
@@ -3441,7 +3432,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D104" s="1" t="s">
         <v>154</v>
       </c>
@@ -3449,7 +3440,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="105" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D105" s="1" t="s">
         <v>155</v>
       </c>
@@ -3457,7 +3448,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="106" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D106" s="1" t="s">
         <v>156</v>
       </c>
@@ -3465,7 +3456,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="108" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D108" s="1" t="s">
         <v>106</v>
       </c>
@@ -3473,7 +3464,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D109" s="1" t="s">
         <v>108</v>
       </c>
@@ -3481,7 +3472,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="110" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D110" s="1" t="s">
         <v>107</v>
       </c>
@@ -3489,7 +3480,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="111" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D111" s="1" t="s">
         <v>157</v>
       </c>
@@ -3497,7 +3488,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>0</v>
       </c>
@@ -3511,7 +3502,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>180</v>
       </c>
@@ -3525,7 +3516,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>161</v>
       </c>
@@ -3539,7 +3530,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>162</v>
       </c>
@@ -3553,7 +3544,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>163</v>
       </c>
@@ -3567,7 +3558,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>164</v>
       </c>
@@ -3581,7 +3572,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>165</v>
       </c>
@@ -3595,7 +3586,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>166</v>
       </c>
@@ -3609,7 +3600,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>167</v>
       </c>
@@ -3623,7 +3614,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>168</v>
       </c>
@@ -3637,7 +3628,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>169</v>
       </c>
@@ -3651,7 +3642,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>170</v>
       </c>
@@ -3665,7 +3656,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>171</v>
       </c>
@@ -3673,7 +3664,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>172</v>
       </c>
@@ -3681,26 +3672,26 @@
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>173</v>
       </c>
+      <c r="B129" s="1" t="s">
+        <v>472</v>
+      </c>
       <c r="D129" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B130" s="1" t="s">
-        <v>471</v>
-      </c>
       <c r="D130" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>179</v>
       </c>
@@ -3714,7 +3705,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>189</v>
       </c>
@@ -3722,7 +3713,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>190</v>
       </c>
@@ -3730,7 +3721,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>191</v>
       </c>
@@ -3738,7 +3729,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>192</v>
       </c>
@@ -3746,7 +3737,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>193</v>
       </c>
@@ -3754,7 +3745,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>194</v>
       </c>
@@ -3762,1252 +3753,1252 @@
         <v>188</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A291" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A295" s="1" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A297" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A299" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A301" s="1" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A303" s="1" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A305" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A307" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A309" s="1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A311" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A313" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A314" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A315" s="1" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A316" s="1" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A317" s="1" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A318" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A319" s="1" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A320" s="1" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A321" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A323" s="1" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A327" s="1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A328" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A329" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A330" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A331" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A332" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A333" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A334" s="1" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A335" s="1" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A336" s="1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A337" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A338" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A339" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A341" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A342" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A343" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A344" s="1" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A345" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A346" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A347" s="1" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A348" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A349" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A350" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A351" s="1" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A353" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A355" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A357" s="1" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A358" s="1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A359" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A360" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A361" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A362" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A363" s="1" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A364" s="1" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A365" s="1" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A366" s="1" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A367" s="1" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A368" s="1" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A369" s="1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A370" s="1" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A371" s="1" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A372" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A373" s="1" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A374" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A375" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A376" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A377" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A378" s="1" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A379" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A380" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A381" s="1" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A382" s="1" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A383" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A384" s="1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A385" s="1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A386" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A387" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A388" s="1" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A389" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A390" s="1" t="s">
         <v>444</v>
       </c>

</xml_diff>

<commit_message>
Add webhook script and service for one-time initialization
</commit_message>
<xml_diff>
--- a/ip assignments.xlsx
+++ b/ip assignments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Foundry\infrastructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC32958-EE5A-447C-B9D8-B048CE56F6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6582ADC-5998-4705-ADDF-E5C353F38C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
   </bookViews>
   <sheets>
     <sheet name="hosts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="252">
   <si>
     <t>#</t>
   </si>
@@ -770,6 +770,12 @@
   </si>
   <si>
     <t>2606:880:0:16</t>
+  </si>
+  <si>
+    <t>wk19</t>
+  </si>
+  <si>
+    <t>10.20.20.124</t>
   </si>
 </sst>
 </file>
@@ -1670,8 +1676,8 @@
   </sheetPr>
   <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="A134" sqref="A134"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2794,6 +2800,14 @@
         <v>129</v>
       </c>
     </row>
+    <row r="107" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D107" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
     <row r="108" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D108" s="1" t="s">
         <v>106</v>

</xml_diff>

<commit_message>
Update readme.md and webhook.sh: correct filesystem count, remove init info, and add IP address wait logic
</commit_message>
<xml_diff>
--- a/ip assignments.xlsx
+++ b/ip assignments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Foundry\infrastructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC83EF7D-288C-4A18-AD6A-1A8BB6888829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EFF0E3-5027-40F0-B100-CFD7A0D1A1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
+    <workbookView xWindow="-28785" yWindow="15" windowWidth="28770" windowHeight="15090" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
   </bookViews>
   <sheets>
     <sheet name="hosts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="248">
   <si>
     <t>#</t>
   </si>
@@ -761,6 +761,9 @@
   </si>
   <si>
     <t xml:space="preserve">10.20.20.199 </t>
+  </si>
+  <si>
+    <t>james</t>
   </si>
 </sst>
 </file>
@@ -1668,8 +1671,8 @@
   </sheetPr>
   <dimension ref="A1:F158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="G102" sqref="G102"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3049,6 +3052,9 @@
       <c r="A140" s="1" t="s">
         <v>211</v>
       </c>
+      <c r="B140" s="1" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">

</xml_diff>

<commit_message>
Enhance UFW configuration for specific IP access, add resetMongo.sh script for MongoDB password management, and implement MikroTik router configuration with comprehensive firewall and routing rules.
</commit_message>
<xml_diff>
--- a/ip assignments.xlsx
+++ b/ip assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Foundry\infrastructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCD3DDB-5530-48AD-AFF9-0AC2EC71CD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6006DD-6C4F-4780-85D5-0859CEBA2AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
   </bookViews>
   <sheets>
     <sheet name="hosts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="260">
   <si>
     <t>#</t>
   </si>
@@ -307,9 +307,6 @@
     <t>Broadcast</t>
   </si>
   <si>
-    <t>Main Site IP</t>
-  </si>
-  <si>
     <t>192.168.0.9</t>
   </si>
   <si>
@@ -754,15 +751,9 @@
     <t>cp3</t>
   </si>
   <si>
-    <t>10.20.20.199</t>
-  </si>
-  <si>
     <t>haproxy lb</t>
   </si>
   <si>
-    <t xml:space="preserve">10.20.20.199 </t>
-  </si>
-  <si>
     <t>james</t>
   </si>
   <si>
@@ -770,6 +761,45 @@
   </si>
   <si>
     <t xml:space="preserve">10.20.10.199 </t>
+  </si>
+  <si>
+    <t>10.20.20.135</t>
+  </si>
+  <si>
+    <t>10.20.20.136</t>
+  </si>
+  <si>
+    <t>mongo1.vm.lan</t>
+  </si>
+  <si>
+    <t>mongo2.vm.lan</t>
+  </si>
+  <si>
+    <t>mongo3.vm.lan</t>
+  </si>
+  <si>
+    <t>192.168.0.136</t>
+  </si>
+  <si>
+    <t>192.168.0.134</t>
+  </si>
+  <si>
+    <t>192.168.0.135</t>
+  </si>
+  <si>
+    <t>Main Site IP #1</t>
+  </si>
+  <si>
+    <t>Main Site IP #2</t>
+  </si>
+  <si>
+    <t>Main Site IP #3</t>
+  </si>
+  <si>
+    <t>10.20.20.67</t>
+  </si>
+  <si>
+    <t>10.20.20.68</t>
   </si>
 </sst>
 </file>
@@ -1675,10 +1705,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F158"/>
+  <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1698,89 +1728,89 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -2185,30 +2215,30 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2342,13 +2372,13 @@
         <v>57</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -2381,16 +2411,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -2412,13 +2442,13 @@
         <v>74</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2437,13 +2467,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>47</v>
@@ -2454,13 +2484,13 @@
         <v>68</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -2468,13 +2498,13 @@
         <v>69</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>69</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -2487,16 +2517,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D68" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -2525,646 +2555,714 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="D72" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="E73" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="D74" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>165</v>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D75" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>76</v>
+      <c r="D76" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D77" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>166</v>
+        <v>101</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>233</v>
+        <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E82" s="1" t="s">
+      <c r="D87" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E87" s="1" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D83" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D84" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D85" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D86" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D87" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D88" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D89" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D90" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D91" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D92" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D93" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>113</v>
+        <v>149</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D94" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D95" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D96" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D97" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D98" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="99" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D99" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="100" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D100" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D101" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="102" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D102" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D103" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="104" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D104" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="105" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D105" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="106" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D106" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="107" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D107" s="1" t="s">
-        <v>230</v>
+        <v>145</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>229</v>
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D108" s="1" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>44</v>
+        <v>122</v>
       </c>
     </row>
     <row r="109" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D109" s="1" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>45</v>
+        <v>123</v>
       </c>
     </row>
     <row r="110" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D110" s="1" t="s">
-        <v>104</v>
+        <v>151</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>46</v>
+        <v>124</v>
       </c>
     </row>
     <row r="111" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D111" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="112" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D112" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D113" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D114" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D115" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D116" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E111" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>242</v>
-      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="D117" s="1" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="D118" s="1" t="s">
-        <v>238</v>
+        <v>105</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>109</v>
+        <v>250</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="D119" s="1" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>110</v>
+        <v>251</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B120" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="D120" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E120" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E120" s="1" t="s">
-        <v>111</v>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125" s="5" t="s">
+      <c r="A125" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="B130" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A126" s="4" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D131" s="4"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B132" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D126" s="4"/>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
+    </row>
+    <row r="149" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B143" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
+    </row>
+    <row r="150" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="145" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
+    <row r="151" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="146" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
+    <row r="152" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="147" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A147" s="2" t="s">
+    <row r="153" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="148" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A148" s="2" t="s">
+    <row r="154" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="149" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A149" s="2" t="s">
+    <row r="155" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="150" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" s="2" t="s">
+    <row r="156" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
+    <row r="157" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="152" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A152" s="2" t="s">
+    <row r="158" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="153" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="2" t="s">
+    <row r="159" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="154" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A154" s="2" t="s">
+    <row r="160" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="155" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="2" t="s">
+    <row r="161" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="156" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
+    <row r="162" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="157" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
+    <row r="163" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
         <v>227</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A158" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove outdated configuration for RB5009 and add new configuration for CCR2116. The RB5009 configuration file has been deleted as it is no longer needed. The new CCR2116 configuration includes updated interface settings, VLAN configurations, DHCP server settings, firewall rules, and routing configurations to enhance network management and security. Additionally, the BGP instance and connection settings have been established for better routing capabilities. This update aims to streamline the network setup and improve overall performance.
</commit_message>
<xml_diff>
--- a/ip assignments.xlsx
+++ b/ip assignments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Foundry\infrastructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6006DD-6C4F-4780-85D5-0859CEBA2AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5C5DBB-78E2-4468-A1EB-B233D7478A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="292">
   <si>
     <t>#</t>
   </si>
@@ -34,15 +34,9 @@
     <t>10.90.90.1</t>
   </si>
   <si>
-    <t>rb5009-1.oob.local</t>
-  </si>
-  <si>
     <t>10.90.90.3</t>
   </si>
   <si>
-    <t>rb5009-2.oob.local</t>
-  </si>
-  <si>
     <t>10.90.90.4</t>
   </si>
   <si>
@@ -199,30 +193,9 @@
     <t>10.20.10.30</t>
   </si>
   <si>
-    <t>rb5009-1.oob.local / rb5009-2.oob.local</t>
-  </si>
-  <si>
-    <t>rb5009-1.mgmt.local / rb5009-2.mgmt.local</t>
-  </si>
-  <si>
     <t>pve3.mgmt.local</t>
   </si>
   <si>
-    <t>spare2.oob.local</t>
-  </si>
-  <si>
-    <t>spare3.oob.local</t>
-  </si>
-  <si>
-    <t>spare2.mgmt.local</t>
-  </si>
-  <si>
-    <t>spare3.mgmt.local</t>
-  </si>
-  <si>
-    <t>caddy1.vm.local</t>
-  </si>
-  <si>
     <t>192.168.0.3</t>
   </si>
   <si>
@@ -310,9 +283,6 @@
     <t>192.168.0.9</t>
   </si>
   <si>
-    <t>monitor1.vm.local</t>
-  </si>
-  <si>
     <t>monitor1.mgmt.local</t>
   </si>
   <si>
@@ -484,9 +454,6 @@
     <t>10.20.20.133</t>
   </si>
   <si>
-    <t>haproxy1.vm.local</t>
-  </si>
-  <si>
     <t>10.20.20.66</t>
   </si>
   <si>
@@ -502,9 +469,6 @@
     <t>Router 1</t>
   </si>
   <si>
-    <t>38.186.49.176/28</t>
-  </si>
-  <si>
     <t>tailscale 2</t>
   </si>
   <si>
@@ -520,18 +484,12 @@
     <t>10.20.20.31</t>
   </si>
   <si>
-    <t>caddy0.vm.local</t>
-  </si>
-  <si>
     <t>Caddy 0</t>
   </si>
   <si>
     <t>Caddy 1</t>
   </si>
   <si>
-    <t>2605:9000:d::300/120</t>
-  </si>
-  <si>
     <t>Subnets In Use</t>
   </si>
   <si>
@@ -577,30 +535,12 @@
     <t>oob no vlan</t>
   </si>
   <si>
-    <t>Public ipv4 vlan 30</t>
-  </si>
-  <si>
-    <t>Public ipv6 vlan 30</t>
-  </si>
-  <si>
-    <t>vmapi0.vm.local</t>
-  </si>
-  <si>
-    <t>vmapi1.vm.local</t>
-  </si>
-  <si>
     <t>10.20.10.6</t>
   </si>
   <si>
     <t>10.20.10.7</t>
   </si>
   <si>
-    <t>vmapi0.mgmt.local</t>
-  </si>
-  <si>
-    <t>vmapi1.mgmt.local</t>
-  </si>
-  <si>
     <t>192.168.0.23</t>
   </si>
   <si>
@@ -742,27 +682,9 @@
     <t>10.20.20.205</t>
   </si>
   <si>
-    <t>cp1</t>
-  </si>
-  <si>
-    <t>cp2</t>
-  </si>
-  <si>
-    <t>cp3</t>
-  </si>
-  <si>
-    <t>haproxy lb</t>
-  </si>
-  <si>
     <t>james</t>
   </si>
   <si>
-    <t>10.20.10.199</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.20.10.199 </t>
-  </si>
-  <si>
     <t>10.20.20.135</t>
   </si>
   <si>
@@ -778,28 +700,202 @@
     <t>mongo3.vm.lan</t>
   </si>
   <si>
+    <t>Main Site IP #1</t>
+  </si>
+  <si>
+    <t>Main Site IP #2</t>
+  </si>
+  <si>
+    <t>Main Site IP #3</t>
+  </si>
+  <si>
+    <t>10.20.20.67</t>
+  </si>
+  <si>
+    <t>10.20.20.68</t>
+  </si>
+  <si>
+    <t>crr2116-1.oob.local / crr2116-2.oob.local</t>
+  </si>
+  <si>
+    <t>crr2116-1.oob.local</t>
+  </si>
+  <si>
+    <t>crr2116-1.mgmt.local / crr2116-2.mgmt.local</t>
+  </si>
+  <si>
+    <t>crr2116-1.oob.lan / crr2116-2.oob.lan</t>
+  </si>
+  <si>
+    <t>crr2116-1.oob.lan</t>
+  </si>
+  <si>
+    <t>crs317-1.oob.lan</t>
+  </si>
+  <si>
+    <t>crs317-2.oob.lan</t>
+  </si>
+  <si>
+    <t>pve0.oob.lan</t>
+  </si>
+  <si>
+    <t>pve1.oob.lan</t>
+  </si>
+  <si>
+    <t>pve2.oob.lan</t>
+  </si>
+  <si>
+    <t>spare2.oob.lan</t>
+  </si>
+  <si>
+    <t>spare3.oob.lan</t>
+  </si>
+  <si>
+    <t>backup1.oob.lan</t>
+  </si>
+  <si>
+    <t>spare0.oob.lan</t>
+  </si>
+  <si>
+    <t>spare1.oob.lan</t>
+  </si>
+  <si>
+    <t>pve3.oob.lan</t>
+  </si>
+  <si>
+    <t>tailscale3.oob.lan</t>
+  </si>
+  <si>
+    <t>tailscale2.oob.lan</t>
+  </si>
+  <si>
+    <t>crr2116-1.mgmt.lan / crr2116-2.mgmt.lan</t>
+  </si>
+  <si>
+    <t>pve0.mgmt.lan</t>
+  </si>
+  <si>
+    <t>pve1.mgmt.lan</t>
+  </si>
+  <si>
+    <t>pve2.mgmt.lan</t>
+  </si>
+  <si>
+    <t>spare2.mgmt.lan</t>
+  </si>
+  <si>
+    <t>spare3.mgmt.lan</t>
+  </si>
+  <si>
+    <t>backup1.mgmt.lan</t>
+  </si>
+  <si>
+    <t>spare0.mgmt.lan</t>
+  </si>
+  <si>
+    <t>spare1.mgmt.lan</t>
+  </si>
+  <si>
+    <t>pve3.mgmt.lan</t>
+  </si>
+  <si>
+    <t>monitor1.mgmt.lan</t>
+  </si>
+  <si>
+    <t>tailscale2.mgmt.lan</t>
+  </si>
+  <si>
+    <t>tailscale1.mgmt.lan</t>
+  </si>
+  <si>
+    <t>caddy0.vm.lan</t>
+  </si>
+  <si>
+    <t>caddy1.vm.lan</t>
+  </si>
+  <si>
+    <t>dev1.vm.lan</t>
+  </si>
+  <si>
+    <t>monitor1.vm.lan</t>
+  </si>
+  <si>
+    <t>199.45.15.0/28</t>
+  </si>
+  <si>
+    <t>Public ipv4 vlan 40</t>
+  </si>
+  <si>
+    <t>Public ipv6 vlan 40</t>
+  </si>
+  <si>
+    <t>192.168.0.1</t>
+  </si>
+  <si>
+    <t>10.20.20.1</t>
+  </si>
+  <si>
+    <t>cp1.vm.lan</t>
+  </si>
+  <si>
+    <t>cp2.vm.lan</t>
+  </si>
+  <si>
+    <t>cp3.vm.lan</t>
+  </si>
+  <si>
+    <t>wk1.vm.lan</t>
+  </si>
+  <si>
+    <t>wk2.vm.lan</t>
+  </si>
+  <si>
+    <t>wk3.vm.lan</t>
+  </si>
+  <si>
+    <t>haproxy1.vm.lan</t>
+  </si>
+  <si>
+    <t>192.168.0.100</t>
+  </si>
+  <si>
+    <t>192.168.0.101</t>
+  </si>
+  <si>
+    <t>192.168.0.102</t>
+  </si>
+  <si>
+    <t>192.168.0.103</t>
+  </si>
+  <si>
+    <t>192.168.0.104</t>
+  </si>
+  <si>
+    <t>192.168.0.105</t>
+  </si>
+  <si>
+    <t>192.168.0.199</t>
+  </si>
+  <si>
     <t>192.168.0.136</t>
   </si>
   <si>
-    <t>192.168.0.134</t>
-  </si>
-  <si>
-    <t>192.168.0.135</t>
-  </si>
-  <si>
-    <t>Main Site IP #1</t>
-  </si>
-  <si>
-    <t>Main Site IP #2</t>
-  </si>
-  <si>
-    <t>Main Site IP #3</t>
-  </si>
-  <si>
-    <t>10.20.20.67</t>
-  </si>
-  <si>
-    <t>10.20.20.68</t>
+    <t>192.168.0.137</t>
+  </si>
+  <si>
+    <t>192.168.0.138</t>
+  </si>
+  <si>
+    <t>metallb dev site dnat ip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.20.10.133 </t>
+  </si>
+  <si>
+    <t>k0sapi.vm.local {ha proxy org k0s}</t>
+  </si>
+  <si>
+    <t>{nodeport1, haproxy1, k0sapi, pve}.vm.lan</t>
   </si>
 </sst>
 </file>
@@ -1705,10 +1801,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F163"/>
+  <dimension ref="A1:F177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1728,89 +1824,89 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>160</v>
+        <v>266</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>185</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>186</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -1848,285 +1944,285 @@
         <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>234</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>59</v>
+        <v>231</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>4</v>
+        <v>235</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>4</v>
+        <v>232</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>235</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>8</v>
+        <v>236</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>10</v>
+        <v>237</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>12</v>
+        <v>238</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>16</v>
+        <v>240</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>241</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>63</v>
+        <v>242</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>243</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>53</v>
+        <v>244</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>23</v>
+        <v>245</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>55</v>
+        <v>247</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>84</v>
+        <v>248</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -2134,293 +2230,275 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>60</v>
+        <v>249</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>60</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="E40" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>30</v>
+        <v>251</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>32</v>
+        <v>252</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>64</v>
+        <v>253</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>65</v>
+        <v>254</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>36</v>
+        <v>255</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>56</v>
+        <v>256</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>40</v>
+        <v>257</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>61</v>
+        <v>258</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>97</v>
+        <v>259</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>42</v>
+        <v>260</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>38</v>
+        <v>261</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="D58" s="1" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>243</v>
+        <v>290</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -2428,841 +2506,814 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>74</v>
+        <v>269</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>166</v>
+        <v>249</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>66</v>
+        <v>262</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D75" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D76" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D77" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>101</v>
+        <v>280</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>76</v>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>165</v>
+        <v>283</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>231</v>
+        <v>276</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>233</v>
+        <v>285</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>155</v>
+        <v>286</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>258</v>
+        <v>287</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D88" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D100" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D101" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D102" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D103" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D104" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D105" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D106" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D107" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D108" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D109" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D110" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E88" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D89" s="1" t="s">
+      <c r="E110" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D111" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E89" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D90" s="1" t="s">
+      <c r="E111" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D112" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D91" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D92" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D93" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D94" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D95" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D96" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D97" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D98" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D99" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D100" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="101" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D101" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="102" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D102" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D103" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D104" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="105" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D105" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="106" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D106" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="107" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D107" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="108" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D108" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="109" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D109" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="110" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D110" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="111" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D111" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="112" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D112" s="1" t="s">
-        <v>229</v>
-      </c>
       <c r="E112" s="1" t="s">
-        <v>228</v>
+        <v>104</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D113" s="1" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D114" s="1" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D115" s="1" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D116" s="1" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D117" s="1" t="s">
-        <v>248</v>
+        <v>133</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D118" s="1" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>250</v>
+        <v>110</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D119" s="1" t="s">
-        <v>247</v>
+        <v>135</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>251</v>
+        <v>111</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="D120" s="1" t="s">
-        <v>234</v>
+        <v>136</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>240</v>
+        <v>112</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="D121" s="1" t="s">
-        <v>235</v>
+        <v>140</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>241</v>
+        <v>113</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>242</v>
-      </c>
       <c r="D122" s="1" t="s">
-        <v>236</v>
+        <v>141</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>242</v>
+        <v>114</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="D123" s="1" t="s">
-        <v>237</v>
+        <v>142</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A124" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="D124" s="1" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="D125" s="1" t="s">
-        <v>239</v>
+        <v>92</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D126" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D127" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B130" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" s="4" t="s">
+      <c r="B144" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D145" s="4"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B131" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D131" s="4"/>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
+    </row>
+    <row r="166" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B132" s="1" t="s">
+    </row>
+    <row r="167" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" s="1" t="s">
+    <row r="168" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B133" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134" s="1" t="s">
+    </row>
+    <row r="169" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135" s="1" t="s">
+    </row>
+    <row r="170" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136" s="1" t="s">
+    </row>
+    <row r="171" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
+    </row>
+    <row r="172" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B137" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
+    </row>
+    <row r="173" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A139" s="1" t="s">
+    </row>
+    <row r="174" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A140" s="1" t="s">
+    </row>
+    <row r="175" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B140" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A141" s="1" t="s">
+    </row>
+    <row r="176" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A142" s="1" t="s">
+    </row>
+    <row r="177" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A143" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A144" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A148" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A149" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A152" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A154" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A158" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A159" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A160" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A161" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove outdated CCR2116 configuration and replace with updated version. The previous configuration file has been deleted, and a new configuration has been added to enhance network management, including updated interface settings, VLAN configurations, and firewall rules.
</commit_message>
<xml_diff>
--- a/ip assignments.xlsx
+++ b/ip assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Foundry\infrastructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9D79C1-3382-4F37-AFA5-E803BC3882FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7507A18-FC72-421B-B99B-BD4AEA8D6810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
   </bookViews>
   <sheets>
     <sheet name="hosts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="276">
   <si>
     <t>#</t>
   </si>
@@ -841,13 +841,13 @@
     <t>k0sapi.vm.local {ha proxy org k0s}</t>
   </si>
   <si>
-    <t>{nodeport1, haproxy1, k0sapi, pve}.vm.lan</t>
-  </si>
-  <si>
     <t>192.168.1.1 - 192.168.255.255</t>
   </si>
   <si>
     <t>haproxy1.vm.local</t>
+  </si>
+  <si>
+    <t>{nodeport, haproxy1, k0sapi, pve}.vm.lan</t>
   </si>
 </sst>
 </file>
@@ -1755,8 +1755,8 @@
   </sheetPr>
   <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="E140" sqref="E140"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2641,24 +2641,18 @@
         <v>266</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="D93" s="1" t="s">
         <v>254</v>
       </c>
@@ -2667,12 +2661,6 @@
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="D94" s="1" t="s">
         <v>151</v>
       </c>
@@ -2681,12 +2669,6 @@
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="D95" s="1" t="s">
         <v>143</v>
       </c>
@@ -2694,13 +2676,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>248</v>
-      </c>
+    <row r="99" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D99" s="1" t="s">
         <v>94</v>
       </c>
@@ -2708,7 +2684,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D100" s="1" t="s">
         <v>115</v>
       </c>
@@ -2716,7 +2692,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D101" s="1" t="s">
         <v>116</v>
       </c>
@@ -2724,7 +2700,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D102" s="1" t="s">
         <v>117</v>
       </c>
@@ -2732,7 +2708,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D103" s="1" t="s">
         <v>118</v>
       </c>
@@ -2740,7 +2716,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D104" s="1" t="s">
         <v>119</v>
       </c>
@@ -2748,7 +2724,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D105" s="1" t="s">
         <v>120</v>
       </c>
@@ -2756,7 +2732,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D106" s="1" t="s">
         <v>121</v>
       </c>
@@ -2764,7 +2740,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D107" s="1" t="s">
         <v>122</v>
       </c>
@@ -2772,7 +2748,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D108" s="1" t="s">
         <v>123</v>
       </c>
@@ -2780,7 +2756,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D109" s="1" t="s">
         <v>124</v>
       </c>
@@ -2788,7 +2764,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D110" s="1" t="s">
         <v>125</v>
       </c>
@@ -2796,7 +2772,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D111" s="1" t="s">
         <v>126</v>
       </c>
@@ -2804,7 +2780,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D112" s="1" t="s">
         <v>127</v>
       </c>
@@ -2937,7 +2913,7 @@
         <v>142</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update ip assignments.xlsx to reflect current network configurations and IP assignments.
</commit_message>
<xml_diff>
--- a/ip assignments.xlsx
+++ b/ip assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Foundry\infrastructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7507A18-FC72-421B-B99B-BD4AEA8D6810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F66A2E-8E52-4F04-B5BD-855AC0119687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
   </bookViews>
   <sheets>
     <sheet name="hosts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="294">
   <si>
     <t>#</t>
   </si>
@@ -838,9 +838,6 @@
     <t xml:space="preserve">10.20.10.133 </t>
   </si>
   <si>
-    <t>k0sapi.vm.local {ha proxy org k0s}</t>
-  </si>
-  <si>
     <t>192.168.1.1 - 192.168.255.255</t>
   </si>
   <si>
@@ -848,6 +845,63 @@
   </si>
   <si>
     <t>{nodeport, haproxy1, k0sapi, pve}.vm.lan</t>
+  </si>
+  <si>
+    <t>10.20.20.200</t>
+  </si>
+  <si>
+    <t>10.20.20.201</t>
+  </si>
+  <si>
+    <t>10.20.20.202</t>
+  </si>
+  <si>
+    <t>10.20.20.203</t>
+  </si>
+  <si>
+    <t>10.20.20.204</t>
+  </si>
+  <si>
+    <t>10.20.20.205</t>
+  </si>
+  <si>
+    <t>10.20.20.206</t>
+  </si>
+  <si>
+    <t>cp-1</t>
+  </si>
+  <si>
+    <t>cp-2</t>
+  </si>
+  <si>
+    <t>cp-3</t>
+  </si>
+  <si>
+    <t>wk-1</t>
+  </si>
+  <si>
+    <t>wk-2</t>
+  </si>
+  <si>
+    <t>wk-3</t>
+  </si>
+  <si>
+    <t>bgp temp IP</t>
+  </si>
+  <si>
+    <t>10.20.10.200</t>
+  </si>
+  <si>
+    <t>k0sapi.mgmt.local {ha proxy org k0s}</t>
+  </si>
+  <si>
+    <t>k0sapi-cilium.mgmt.local {ha proxy cilium k0s}</t>
+  </si>
+  <si>
+    <t>10.20.10.136</t>
+  </si>
+  <si>
+    <t>dev1.mgmt.local</t>
   </si>
 </sst>
 </file>
@@ -1753,10 +1807,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F163"/>
+  <dimension ref="A1:F174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G113" sqref="G113"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1765,7 +1819,7 @@
     <col min="2" max="2" width="45" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="20.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="45" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -2447,677 +2501,752 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D58" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D59" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>272</v>
+      <c r="E59" s="1" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D60" s="1" t="s">
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>41</v>
+        <v>291</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>253</v>
+        <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>246</v>
+        <v>41</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>58</v>
+        <v>253</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>60</v>
+        <v>90</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>249</v>
+        <v>60</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>172</v>
+        <v>63</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>147</v>
+        <v>64</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>150</v>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>260</v>
+        <v>149</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>256</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>212</v>
+        <v>259</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D93" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D94" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D95" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D96" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D97" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D99" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D100" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="101" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D101" s="1" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D102" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
     </row>
     <row r="103" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D103" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="104" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D104" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>137</v>
+        <v>96</v>
       </c>
     </row>
     <row r="105" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D105" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D106" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
     </row>
     <row r="107" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D107" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
     </row>
     <row r="108" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D108" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="109" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D109" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="110" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D110" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="111" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D111" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="112" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D112" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="113" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D113" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="114" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D114" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="115" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D115" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="116" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D116" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="117" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D117" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="118" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D118" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="119" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D119" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="120" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D120" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="121" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D121" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="122" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D122" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="123" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D123" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="124" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D124" s="1" t="s">
-        <v>207</v>
+        <v>140</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>206</v>
+        <v>113</v>
       </c>
     </row>
     <row r="125" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D125" s="1" t="s">
-        <v>91</v>
+        <v>141</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
     </row>
     <row r="126" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D126" s="1" t="s">
-        <v>93</v>
+        <v>207</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>43</v>
+        <v>206</v>
       </c>
     </row>
     <row r="127" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D127" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="128" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D128" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D129" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D130" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E128" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" s="5" t="s">
+      <c r="E130" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D132" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D133" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D134" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D135" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D136" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D137" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D138" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B130" s="5" t="s">
+      <c r="B141" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" s="4" t="s">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B142" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D131" s="4"/>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
+      <c r="D142" s="4"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B143" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" s="1" t="s">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B144" s="1" t="s">
         <v>214</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A139" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A140" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A141" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A142" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A143" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A144" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>210</v>
+        <v>144</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B157" s="1" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A148" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A149" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A152" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A154" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A158" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>201</v>
+        <v>190</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
         <v>205</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update RADOS Gateway documentation to include user and bucket creation instructions
- Added commands for creating users and buckets using radosgw-admin and AWS CLI.
- Improved section title for clarity.
</commit_message>
<xml_diff>
--- a/ip assignments.xlsx
+++ b/ip assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Foundry\infrastructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF442D0-A38D-450D-A51E-FFAEA12995D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D95746F-DBF4-4C60-9376-A8364C9CBD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="236">
   <si>
     <t>#</t>
   </si>
@@ -679,9 +679,6 @@
     <t>CRR317 Router</t>
   </si>
   <si>
-    <t>Development IP</t>
-  </si>
-  <si>
     <t>NFS 1</t>
   </si>
   <si>
@@ -689,6 +686,48 @@
   </si>
   <si>
     <t>Public ipv6 vlan 41</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>10.20.30.20</t>
+  </si>
+  <si>
+    <t>pve0 - ceph</t>
+  </si>
+  <si>
+    <t>10.20.30.21</t>
+  </si>
+  <si>
+    <t>10.20.30.22</t>
+  </si>
+  <si>
+    <t>10.20.30.28</t>
+  </si>
+  <si>
+    <t>pve1 - ceph</t>
+  </si>
+  <si>
+    <t>pve2 - ceph</t>
+  </si>
+  <si>
+    <t>pve3 - ceph</t>
+  </si>
+  <si>
+    <t>Development IP ( s3 )</t>
+  </si>
+  <si>
+    <t>Development IP ( sftp )</t>
+  </si>
+  <si>
+    <t>Development IP ( gateway api )</t>
+  </si>
+  <si>
+    <t>10.20.30.254</t>
+  </si>
+  <si>
+    <t>dev 1</t>
   </si>
 </sst>
 </file>
@@ -1222,11 +1261,11 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1607,8 +1646,8 @@
   </sheetPr>
   <dimension ref="A1:F210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1668,19 +1707,19 @@
         <v>130</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -1720,7 +1759,7 @@
         <v>117</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1731,7 +1770,7 @@
         <v>118</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1760,6 +1799,9 @@
       <c r="A17" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="B17" s="6" t="s">
+        <v>233</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1768,6 +1810,9 @@
       <c r="A18" s="1" t="s">
         <v>122</v>
       </c>
+      <c r="B18" s="6" t="s">
+        <v>231</v>
+      </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1776,8 +1821,8 @@
       <c r="A19" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>219</v>
+      <c r="B19" s="6" t="s">
+        <v>232</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1787,7 +1832,7 @@
       <c r="A20" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B20" s="7"/>
+      <c r="B20" s="6"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -1796,7 +1841,7 @@
       <c r="A21" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B21" s="7"/>
+      <c r="B21" s="6"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1805,7 +1850,7 @@
       <c r="A22" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1814,7 +1859,7 @@
       <c r="A23" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="7"/>
+      <c r="B23" s="6"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1823,7 +1868,7 @@
       <c r="A24" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="7"/>
+      <c r="B24" s="6"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -1855,10 +1900,10 @@
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2047,10 +2092,10 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2209,10 +2254,10 @@
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="8" t="s">
+      <c r="A71" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="B71" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2561,6 +2606,54 @@
       </c>
       <c r="B119" s="1" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A122" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add S3 bucket lifecycle configuration guide and JSON policy file
- Introduced a new section in the RADOS Gateway documentation detailing S3 bucket lifecycle configuration, including auto-expiration policies and management.
- Added a JSON file for lifecycle policy that enables automatic deletion of objects after 31 days.
</commit_message>
<xml_diff>
--- a/ip assignments.xlsx
+++ b/ip assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Foundry\infrastructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D95746F-DBF4-4C60-9376-A8364C9CBD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A32CBB-1EE8-4D33-9DF4-02169B76DD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="243">
   <si>
     <t>#</t>
   </si>
@@ -313,9 +313,6 @@
     <t>wk18</t>
   </si>
   <si>
-    <t>10.20.20.66</t>
-  </si>
-  <si>
     <t>sftp1</t>
   </si>
   <si>
@@ -355,12 +352,6 @@
     <t>oob no vlan</t>
   </si>
   <si>
-    <t>10.20.10.6</t>
-  </si>
-  <si>
-    <t>10.20.10.7</t>
-  </si>
-  <si>
     <t>199.45.150.0/28</t>
   </si>
   <si>
@@ -619,9 +610,6 @@
     <t>10.20.20.67</t>
   </si>
   <si>
-    <t>Dev NAT IP</t>
-  </si>
-  <si>
     <t>10.20.20.207</t>
   </si>
   <si>
@@ -670,15 +658,9 @@
     <t>199.45.150.0</t>
   </si>
   <si>
-    <t>Beanfield Gateway</t>
-  </si>
-  <si>
     <t>Production IP</t>
   </si>
   <si>
-    <t>CRR317 Router</t>
-  </si>
-  <si>
     <t>NFS 1</t>
   </si>
   <si>
@@ -728,6 +710,45 @@
   </si>
   <si>
     <t>dev 1</t>
+  </si>
+  <si>
+    <t>96.45.201.62/30</t>
+  </si>
+  <si>
+    <t>96.45.201.60</t>
+  </si>
+  <si>
+    <t>96.45.201.61</t>
+  </si>
+  <si>
+    <t>96.45.201.62</t>
+  </si>
+  <si>
+    <t>96.45.201.63</t>
+  </si>
+  <si>
+    <t>Foundry Gateway</t>
+  </si>
+  <si>
+    <t>Foundry ( P2P )</t>
+  </si>
+  <si>
+    <t>Beanfield ( P2P )</t>
+  </si>
+  <si>
+    <t>10.20.10.60</t>
+  </si>
+  <si>
+    <t>influxdb</t>
+  </si>
+  <si>
+    <t>10.20.20.60</t>
+  </si>
+  <si>
+    <t>P2P With Beanfield vlan 50</t>
+  </si>
+  <si>
+    <t>Production IP ( gateway api)</t>
   </si>
 </sst>
 </file>
@@ -1644,10 +1665,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F210"/>
+  <dimension ref="A1:F213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1667,47 +1688,55 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1723,7 +1752,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>72</v>
@@ -1734,10 +1763,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>114</v>
+        <v>232</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>216</v>
+        <v>237</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1745,10 +1774,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>116</v>
+        <v>233</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1756,29 +1785,28 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>117</v>
+        <v>234</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>219</v>
+        <v>73</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>220</v>
-      </c>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>119</v>
+        <v>211</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1786,10 +1814,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>218</v>
+        <v>235</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1797,10 +1825,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>233</v>
+        <v>113</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1808,10 +1836,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>231</v>
+        <v>114</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1819,10 +1847,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>232</v>
+        <v>115</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1830,1042 +1858,1091 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B20" s="6"/>
+        <v>116</v>
+      </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B21" s="6"/>
+        <v>117</v>
+      </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B22" s="6"/>
+        <v>118</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>227</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B23" s="6"/>
+        <v>119</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>225</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B24" s="6"/>
+        <v>120</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>226</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>73</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="B25" s="6"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="6"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="6"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="6"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>1</v>
-      </c>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B35" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="B36" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B37" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>35</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>210</v>
+        <v>54</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>158</v>
+        <v>206</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>101</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>97</v>
+        <v>202</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>188</v>
+        <v>240</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>212</v>
+        <v>239</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>160</v>
+        <v>209</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>79</v>
+        <v>156</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>80</v>
+        <v>157</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>81</v>
+        <v>184</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>75</v>
+        <v>182</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>77</v>
+        <v>183</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>43</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>202</v>
+        <v>77</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>148</v>
+        <v>42</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>150</v>
+        <v>43</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="3"/>
+      <c r="A109" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>161</v>
+        <v>78</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>211</v>
+        <v>146</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>162</v>
+        <v>199</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>169</v>
-      </c>
+      <c r="A112" s="3"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>201</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A122" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A125" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B122" s="7" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>229</v>
+      <c r="B125" s="7" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B180" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B178" s="1" t="s">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B181" s="1" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A181" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>174</v>
+        <v>97</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B193" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B196" s="1" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A195" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A196" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A197" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="209" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="210" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A30:C46">
-    <sortCondition ref="A30:A46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:C51">
+    <sortCondition ref="A35:A51"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="D9:F9"/>

</xml_diff>

<commit_message>
Update IP assignments spreadsheet with new entries
</commit_message>
<xml_diff>
--- a/ip assignments.xlsx
+++ b/ip assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Foundry\infrastructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A32CBB-1EE8-4D33-9DF4-02169B76DD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F15EFA3-FC71-46B4-AD97-72DEB63DA7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0F35F731-BE1A-4568-B0B3-67870C25BC91}"/>
   </bookViews>
   <sheets>
     <sheet name="hosts" sheetId="1" r:id="rId1"/>
@@ -658,9 +658,6 @@
     <t>199.45.150.0</t>
   </si>
   <si>
-    <t>Production IP</t>
-  </si>
-  <si>
     <t>NFS 1</t>
   </si>
   <si>
@@ -697,9 +694,6 @@
     <t>pve3 - ceph</t>
   </si>
   <si>
-    <t>Development IP ( s3 )</t>
-  </si>
-  <si>
     <t>Development IP ( sftp )</t>
   </si>
   <si>
@@ -727,9 +721,6 @@
     <t>96.45.201.63</t>
   </si>
   <si>
-    <t>Foundry Gateway</t>
-  </si>
-  <si>
     <t>Foundry ( P2P )</t>
   </si>
   <si>
@@ -749,6 +740,15 @@
   </si>
   <si>
     <t>Production IP ( gateway api)</t>
+  </si>
+  <si>
+    <t>Development Egress Ip Gateway</t>
+  </si>
+  <si>
+    <t>Production Egress IP Gateway</t>
+  </si>
+  <si>
+    <t>Foundry Gateway  on Router</t>
   </si>
 </sst>
 </file>
@@ -1668,7 +1668,7 @@
   <dimension ref="A1:F213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1728,15 +1728,15 @@
         <v>127</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1752,7 +1752,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>72</v>
@@ -1763,10 +1763,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1774,10 +1774,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1785,7 +1785,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>73</v>
@@ -1817,7 +1817,7 @@
         <v>111</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1827,100 +1827,97 @@
       <c r="A17" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>212</v>
-      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="E18"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="E19"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>116</v>
       </c>
       <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="E20"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>117</v>
       </c>
       <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="E21"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="E22"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="E23"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="E24"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B25" s="6"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="E25"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B26" s="6"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="E26"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1936,7 +1933,9 @@
       <c r="A28" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="6"/>
+      <c r="B28" s="6" t="s">
+        <v>241</v>
+      </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -1946,7 +1945,7 @@
         <v>125</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -2316,10 +2315,10 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -2372,10 +2371,10 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -2690,47 +2689,47 @@
         <v>0</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>